<commit_message>
Uploading starter code file to repository for team
</commit_message>
<xml_diff>
--- a/Project Ideation/Data Science Bootcamp Project #1 Plan_vShare.xlsx
+++ b/Project Ideation/Data Science Bootcamp Project #1 Plan_vShare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lexis\class\project-1-northwestern-bootcamp\Project Ideation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{317D85FA-B611-48FA-91E8-2D7270902ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B90744-8BCA-4624-8121-E5D1751D4C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9672" yWindow="0" windowWidth="13380" windowHeight="12336" xr2:uid="{E33CEE9D-08E5-4CAA-BBB8-17D332833924}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E33CEE9D-08E5-4CAA-BBB8-17D332833924}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Activity</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>Est. Completion</t>
-  </si>
-  <si>
     <t>Setup the project</t>
   </si>
   <si>
@@ -168,6 +165,15 @@
   </si>
   <si>
     <t>May not have data available</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -225,16 +231,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -577,12 +582,12 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A11" sqref="A11:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -595,268 +600,278 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4">
         <v>45392</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>45396</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="5">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4">
         <v>45395</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>45396</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
         <v>45395</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>45396</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="5">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4">
         <v>45395</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>45396</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
         <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="5">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="4">
         <v>45396</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
         <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>